<commit_message>
The excel sheet that used for listing is protected
</commit_message>
<xml_diff>
--- a/public/assets/files/Register Collectors.xlsx
+++ b/public/assets/files/Register Collectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MOH-Payment-OTC-System\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA86684-3755-4077-8E43-0748992AF0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A3E4E-4BD2-4D4D-B0D4-CED45343A573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{0C6F8C5F-C272-4CDB-A591-8A9AF8629037}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +603,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="2ZtuOoxjoyIz78SaCxP22EB8FsuxwI45UwQMrHYpuuqjecmjn1n5Ou/aImNKrLMwlGaXu1lVE1s+at6S9eBoWA==" saltValue="TysL762dcllsvX6lXzu1NQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>